<commit_message>
commit baru 2025 08
</commit_message>
<xml_diff>
--- a/dataset/faq.xlsx
+++ b/dataset/faq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dara\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73647BF9-5219-4436-A0C4-81CF3CF9AED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB13C79-AA74-49FB-AD18-B4464CA42605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9936A992-2DCE-420E-95DC-4F7B900A3A30}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>no</t>
   </si>
@@ -51,9 +51,6 @@
     <t>DARA adalah aplikasi yang dirancang untuk menganalisis respons dan aspirasi masyarakat terhadap pengaduan dan ulasan layanan rumah sakit. Aplikasi ini membantu pihak rumah sakit dan instansi terkait untuk memahami topik dan sentimen dari ulasan pengguna sehingga dapat meningkatkan kualitas layanan.</t>
   </si>
   <si>
-    <t>Apa saja fitur utama yang disediakan oleh DARA?</t>
-  </si>
-  <si>
     <t>Siapa yang dapat menggunakan Aplikasi DARA?</t>
   </si>
   <si>
@@ -78,23 +75,16 @@
     <t>Apakah DARA mendukung integrasi dengan sistem lain?</t>
   </si>
   <si>
-    <t>Ya, DARA dapat diintegrasikan dengan sistem informasi rumah sakit (SIRS) atau platform lain melalui API yang tersedia.</t>
-  </si>
-  <si>
-    <t>Apa manfaat utama menggunakan DARA?</t>
-  </si>
-  <si>
     <t>Bagaimana cara memberikan masukan atau melaporkan masalah terkait DARA?</t>
   </si>
   <si>
-    <t>Anda dapat menghubungi tim dukungan pelanggan DARA melalui email: support@dara.com.com atau mengisi formulir kontak di situs resmi aplikasi.</t>
-  </si>
-  <si>
-    <t>Analisis Topik: Mengelompokkan ulasan berdasarkan topik tertentu seperti fasilitas, pelayanan dokter, atau kebersihan \n
-Analisis Sentimen</t>
-  </si>
-  <si>
     <t>Manajemen rumah sakit, Instansi pemerintah yang terkait dengan layanan kesehatan, Peneliti dan akademisi yang mempelajari layanan publik</t>
+  </si>
+  <si>
+    <t>Anda dapat menghubungi tim dukungan pelanggan DARA melalui email: layanan.dara@gmail.com.com atau mengisi formulir kontak di situs resmi aplikasi.</t>
+  </si>
+  <si>
+    <t>Ya, DARA dapat diintegrasikan dengan sistem informasi rumah sakit (SIMRS) atau platform lain melalui API yang tersedia.</t>
   </si>
 </sst>
 </file>
@@ -138,21 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749865DD-3086-4A50-984C-4D7BF5ADB3D1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,15 +479,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
+      <c r="C3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -520,7 +498,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -528,10 +506,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -539,10 +517,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -550,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -564,27 +542,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>